<commit_message>
Implemented Doubly Linked Lists
Implemented Doubly Linked List which performs insertion at end, insertion at beginning, reversing by both itarative and recursive method
</commit_message>
<xml_diff>
--- a/DS and Algo Practice/DS Algo Question Bank.xlsx
+++ b/DS and Algo Practice/DS Algo Question Bank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaunak\Documents\Computer Science\Coding\DS and Algo Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D656770-3131-42DA-9BD3-0BD84085BE62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D985CDD-FFC1-4162-AE95-23FA77A69B2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2096,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D141" sqref="D141"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>